<commit_message>
archivos excel preguntas moderadas
</commit_message>
<xml_diff>
--- a/src/assets/documents/preguntaObjetivasConservador.xlsx
+++ b/src/assets/documents/preguntaObjetivasConservador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sullc\Documents\TPI\Workspace\TPIntegrador\Angular\TPI-Front\src\assets\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9578752-FB73-4770-B604-1CA4E29DDF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8C97CC-D33F-4C3F-A74E-87D69A922767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" activeTab="2" xr2:uid="{EA040AEE-35B0-4F5B-AEF3-29BB44B005B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{EA040AEE-35B0-4F5B-AEF3-29BB44B005B2}"/>
   </bookViews>
   <sheets>
     <sheet name="categoria" sheetId="1" r:id="rId1"/>
@@ -598,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67F1D32-4EEB-430C-A9B4-3504E8B95258}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -687,7 +687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E557A189-07BD-4DD4-AE4E-E2A608F405F0}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -2212,23 +2212,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100641454CD1F1E6E428D478A5DC37BACE7" ma:contentTypeVersion="8" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ef1708d85dca7377bd826ec35b62ca84">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9" xmlns:ns4="7798dcc9-908f-468f-826a-c598f412d6fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="69e720de7d55d3231f99e1910e4c19d8" ns3:_="" ns4:_="">
     <xsd:import namespace="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9"/>
@@ -2417,32 +2400,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46D3E674-3079-48B5-BFCB-0E49FE180026}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7798dcc9-908f-468f-826a-c598f412d6fc"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FE838D2-67DD-483F-BECE-425D67F53E63}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7274836D-657B-48C7-97FD-AD88493854E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2459,4 +2434,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FE838D2-67DD-483F-BECE-425D67F53E63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46D3E674-3079-48B5-BFCB-0E49FE180026}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7798dcc9-908f-468f-826a-c598f412d6fc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87ddcb0d-d42d-44d1-b07a-22e3752ef0c9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>